<commit_message>
data of mean prices per year
</commit_message>
<xml_diff>
--- a/CPI2.xlsx
+++ b/CPI2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15280" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1120" windowWidth="28160" windowHeight="15280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,10 +341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,11 +474,6 @@
         <v>115.333198124109</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>120.540852639769</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
regression of prices as a function of catch
</commit_message>
<xml_diff>
--- a/CPI2.xlsx
+++ b/CPI2.xlsx
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>cpi</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -341,136 +344,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>1990</v>
+      </c>
+      <c r="B2">
         <v>8.5544159743032395</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>1991</v>
+      </c>
+      <c r="B3">
         <v>11.010330701559001</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>1992</v>
+      </c>
+      <c r="B4">
         <v>13.4092895487289</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>1993</v>
+      </c>
+      <c r="B5">
         <v>14.720912024188401</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>1994</v>
+      </c>
+      <c r="B6">
         <v>16.713276338199002</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>1995</v>
+      </c>
+      <c r="B7">
         <v>20.588957549981</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>1996</v>
+      </c>
+      <c r="B8">
         <v>24.196656518752899</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>1997</v>
+      </c>
+      <c r="B9">
         <v>27.3982298355733</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>1998</v>
+      </c>
+      <c r="B10">
         <v>30.594532941416599</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>1999</v>
+      </c>
+      <c r="B11">
         <v>33.668024161160503</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>2000</v>
+      </c>
+      <c r="B12">
         <v>37.368989893888298</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>2001</v>
+      </c>
+      <c r="B13">
         <v>41.564397238272399</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>2002</v>
+      </c>
+      <c r="B14">
         <v>45.373697680273601</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>2003</v>
+      </c>
+      <c r="B15">
         <v>49.660407175345902</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>2004</v>
+      </c>
+      <c r="B16">
         <v>55.776101677506396</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>2005</v>
+      </c>
+      <c r="B17">
         <v>63.472074398945502</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>2006</v>
+      </c>
+      <c r="B18">
         <v>70.752658185494994</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
+        <v>2007</v>
+      </c>
+      <c r="B19">
         <v>77.373218876972501</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>2008</v>
+      </c>
+      <c r="B20">
         <v>87.759301763321105</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>2009</v>
+      </c>
+      <c r="B21">
         <v>94.642988552689303</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
+        <v>2010</v>
+      </c>
+      <c r="B22">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>2011</v>
+      </c>
+      <c r="B23">
         <v>104.88301248136899</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
+        <v>2012</v>
+      </c>
+      <c r="B24">
         <v>109.60701436092801</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
+        <v>2013</v>
+      </c>
+      <c r="B25">
         <v>115.333198124109</v>
       </c>
     </row>

</xml_diff>